<commit_message>
Chooser for Browser Done
</commit_message>
<xml_diff>
--- a/Training_Result.xlsx
+++ b/Training_Result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10185" windowHeight="9090" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="10185" windowHeight="9090" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="299">
   <si>
     <t>sameratio_keepform_32 (SK)</t>
   </si>
@@ -504,6 +504,27 @@
     <t>45m 13s</t>
   </si>
   <si>
+    <t>El-Shawy epoch 128 bs 64</t>
+  </si>
+  <si>
+    <t>86.81</t>
+  </si>
+  <si>
+    <t>88.24</t>
+  </si>
+  <si>
+    <t>83.82</t>
+  </si>
+  <si>
+    <t>83.91 +/- 3.41</t>
+  </si>
+  <si>
+    <t>1h 18m 36s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El Shawy Graph is converge now</t>
+  </si>
+  <si>
     <t>sameratio_diffform_32 (MODORI_SD)</t>
   </si>
   <si>
@@ -573,6 +594,21 @@
     <t>lowest r</t>
   </si>
   <si>
+    <t>macro p</t>
+  </si>
+  <si>
+    <t>macro r</t>
+  </si>
+  <si>
+    <t>weighted p</t>
+  </si>
+  <si>
+    <t>weighted r</t>
+  </si>
+  <si>
+    <t>n parameter</t>
+  </si>
+  <si>
     <t>DK f=6 BoW</t>
   </si>
   <si>
@@ -597,6 +633,12 @@
     <t>0.88</t>
   </si>
   <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
     <t>SK f=6 BoW</t>
   </si>
   <si>
@@ -618,6 +660,9 @@
     <t>0.83</t>
   </si>
   <si>
+    <t>0.96</t>
+  </si>
+  <si>
     <t>DD f=6 BoW</t>
   </si>
   <si>
@@ -663,9 +708,27 @@
     <t>0.81</t>
   </si>
   <si>
+    <t>0.95</t>
+  </si>
+  <si>
     <t>DD f=8 BoW</t>
   </si>
   <si>
+    <t>89.74</t>
+  </si>
+  <si>
+    <t>90.81</t>
+  </si>
+  <si>
+    <t>95.08 +/- 4.15</t>
+  </si>
+  <si>
+    <t>1h 28m</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
     <t>93.41</t>
   </si>
   <si>
@@ -678,6 +741,42 @@
     <t>1h 33m</t>
   </si>
   <si>
+    <t>DK f=8 WoB</t>
+  </si>
+  <si>
+    <t>75.82</t>
+  </si>
+  <si>
+    <t>90.07</t>
+  </si>
+  <si>
+    <t>91.41 +/- 8.41</t>
+  </si>
+  <si>
+    <t>1h 25m 11s</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>DK f=8 BoW</t>
+  </si>
+  <si>
+    <t>93.77</t>
+  </si>
+  <si>
+    <t>97.65 +/- 2.12</t>
+  </si>
+  <si>
+    <t>1h 23m 52 s</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
     <t>DD f=32 WoB</t>
   </si>
   <si>
@@ -711,7 +810,7 @@
     <t>4h 34m 45s</t>
   </si>
   <si>
-    <t>DK f32 BoW</t>
+    <t>DK f=32 BoW</t>
   </si>
   <si>
     <t>96.63</t>
@@ -723,9 +822,6 @@
     <t>4h 44m 52s</t>
   </si>
   <si>
-    <t>0.71</t>
-  </si>
-  <si>
     <t>0.77</t>
   </si>
   <si>
@@ -742,6 +838,81 @@
   </si>
   <si>
     <t>0.19</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>DK f=4 BoW</t>
+  </si>
+  <si>
+    <t>88.64</t>
+  </si>
+  <si>
+    <t>93.38</t>
+  </si>
+  <si>
+    <t>95.01 +/- 3.66</t>
+  </si>
+  <si>
+    <t>1h 10m 7s</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>DD f=4 BoW</t>
+  </si>
+  <si>
+    <t>90.84</t>
+  </si>
+  <si>
+    <t>95.89 +/- 3.33</t>
+  </si>
+  <si>
+    <t>1h 13m 26s</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>DK f=16 BoW</t>
+  </si>
+  <si>
+    <t>94.65 +/- 6.50</t>
+  </si>
+  <si>
+    <t>2h 13m 22s</t>
+  </si>
+  <si>
+    <t>DD f=16 BoW</t>
+  </si>
+  <si>
+    <t>96.40 +/- 3.01</t>
+  </si>
+  <si>
+    <t>2h 27m 7s</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.70</t>
   </si>
 </sst>
 </file>
@@ -750,8 +921,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -776,8 +947,39 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -791,49 +993,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -846,14 +1009,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -869,6 +1032,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -876,25 +1062,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -912,11 +1083,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -941,7 +1112,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -953,37 +1238,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,133 +1292,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,27 +1321,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1186,16 +1355,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1217,24 +1386,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1252,152 +1423,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1432,6 +1603,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1755,7 +1932,7 @@
   <sheetPr/>
   <dimension ref="A2:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2396,10 +2573,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2806,21 +2983,42 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H18" s="1">
+        <v>81</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J18" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2862,28 +3060,28 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="H21" s="6">
         <v>63</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2891,28 +3089,28 @@
         <v>25</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="H22" s="6">
         <v>63</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2920,28 +3118,28 @@
         <v>32</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H23" s="10">
         <v>55</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2970,25 +3168,27 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:K32"/>
+  <dimension ref="A2:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
     <col min="2" max="6" width="7.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="10" max="15" width="9" style="1"/>
+    <col min="16" max="16" width="9.375" style="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
       <c r="B2" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2997,7 +3197,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:16">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3023,21 +3223,36 @@
         <v>8</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>191</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>58</v>
@@ -3046,92 +3261,137 @@
         <v>51</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="H4" s="6">
         <v>98</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>204</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="P4" s="13">
+        <v>320897</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="3" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="H5" s="6">
         <v>96</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="J5" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="P5" s="13">
+        <v>320897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="H6" s="6">
         <v>96</v>
       </c>
       <c r="I6" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="J6" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>206</v>
+      <c r="M6" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="P6" s="13">
+        <v>320897</v>
       </c>
     </row>
     <row r="8" spans="8:8">
@@ -3139,7 +3399,7 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="2" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3148,7 +3408,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3174,410 +3434,913 @@
         <v>8</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>191</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="3" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="H12" s="6">
         <v>95</v>
       </c>
       <c r="I12" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="P12" s="13">
+        <v>528310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="4">
+        <v>100</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="H13" s="6">
+        <v>97</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="P13" s="13">
+        <v>528310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H14" s="8">
+        <v>95</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="P14" s="13">
+        <v>528310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="5">
+        <v>100</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="H15" s="8">
+        <v>96</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="P15" s="13">
+        <v>528310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H16" s="8">
+        <v>94</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K16" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="P16" s="13">
+        <v>528310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H17" s="6">
+        <v>96</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="P17" s="13">
+        <v>7065820</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H18" s="9">
+        <v>97</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="P18" s="13">
+        <v>7065820</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="H19" s="10">
+        <v>94</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="P19" s="13">
+        <v>7065820</v>
+      </c>
+    </row>
+    <row r="20" spans="12:16">
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="J21" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="6">
+        <v>80</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M22" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="N22" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="P22" s="13">
+        <v>320897</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="4">
+        <v>100</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="6">
+        <v>95</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="L23" s="12" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="3" t="s">
+      <c r="M23" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="P23" s="13">
+        <v>320897</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="4">
+        <v>100</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="6">
+        <v>96</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="P24" s="13">
+        <v>320897</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="6">
+        <v>47</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="P25" s="13">
+        <v>320897</v>
+      </c>
+    </row>
+    <row r="26" spans="10:11">
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H27" s="6">
+        <v>92</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="P27" s="13">
+        <v>166123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="H28" s="6">
+        <v>93</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="P28" s="13">
+        <v>166123</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F30" s="4">
+        <v>100</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="H30" s="6">
+        <v>95</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="P30" s="13">
+        <v>1876168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D31" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H13" s="8">
-        <v>95</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="H14" s="6">
-        <v>96</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="H15" s="9">
-        <v>97</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="H16" s="10">
-        <v>94</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="J18" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="6">
-        <v>80</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="4">
-        <v>100</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="6">
-        <v>95</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="4">
-        <v>100</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="6">
-        <v>96</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22" s="6">
-        <v>47</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="10:11">
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-    </row>
-    <row r="24" spans="8:8">
-      <c r="H24" s="7"/>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="2:9">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" ht="15" spans="1:9">
-      <c r="A28" s="3"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-    </row>
-    <row r="29" ht="15" spans="1:9">
-      <c r="A29" s="3"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-    </row>
-    <row r="30" ht="15" spans="1:9">
-      <c r="A30" s="3"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-    </row>
-    <row r="32" spans="8:8">
-      <c r="H32" s="7"/>
+      <c r="G31" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="H31" s="6">
+        <v>93</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="P31" s="13">
+        <v>1876168</v>
+      </c>
+    </row>
+    <row r="32" ht="15" spans="1:16">
+      <c r="A32" s="3"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+    </row>
+    <row r="33" ht="15" spans="1:16">
+      <c r="A33" s="3"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+    </row>
+    <row r="35" spans="8:8">
+      <c r="H35" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B29:H29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>